<commit_message>
Set up spike detection for pre- and post-SALPA
</commit_message>
<xml_diff>
--- a/metadata/mecp2RecordingsListNew.xlsx
+++ b/metadata/mecp2RecordingsListNew.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATLAB\MEA-NAP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATLAB\MEA-NAP\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BD063D-096E-4473-9B58-0DB8CD7D0E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0F7878-0B9E-4AE2-82E9-A665B075BC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{CE5D0629-84EA-4DEB-B886-7B072FA3D434}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{CE5D0629-84EA-4DEB-B886-7B072FA3D434}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="106">
   <si>
     <t>231101_Mutant_ALICO3_1_Baseline</t>
   </si>
@@ -1859,10 +1859,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF1FF9A-91A7-4CC9-B549-87D7B9661614}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="129" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A15"/>
+    <sheetView tabSelected="1" zoomScale="129" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1888,7 +1888,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4">
         <v>150</v>
@@ -1903,7 +1903,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="4">
         <v>150</v>
@@ -1918,13 +1918,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4">
         <v>150</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D4" s="4">
         <v>15</v>
@@ -1933,7 +1933,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" s="4">
         <v>150</v>
@@ -1948,13 +1948,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B6" s="4">
         <v>150</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
       <c r="D6" s="4">
         <v>15</v>
@@ -1963,13 +1963,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="B7" s="4">
         <v>150</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
       <c r="D7" s="4">
         <v>15</v>
@@ -1978,67 +1978,69 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B8" s="4">
         <v>150</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="4">
-        <v>15</v>
+        <v>70</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B9" s="4">
         <v>150</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="4">
-        <v>15</v>
-      </c>
-      <c r="E9" s="4"/>
+        <v>70</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="B10" s="4">
         <v>150</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="4">
-        <v>15</v>
+        <v>69</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B11" s="4">
         <v>150</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B12" s="4">
         <v>150</v>
@@ -2053,13 +2055,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B13" s="4">
         <v>150</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>76</v>
@@ -2068,7 +2070,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="B14" s="4">
         <v>150</v>
@@ -2083,7 +2085,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B15" s="4">
         <v>150</v>
@@ -2094,13 +2096,11 @@
       <c r="D15" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B16" s="4">
         <v>150</v>
@@ -2109,15 +2109,13 @@
         <v>69</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>84</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>39</v>
+        <v>86</v>
       </c>
       <c r="B17" s="4">
         <v>150</v>
@@ -2126,49 +2124,49 @@
         <v>69</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="B18" s="4">
         <v>150</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4">
         <v>150</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="B20" s="4">
         <v>150</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>76</v>
@@ -2177,13 +2175,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="B21" s="4">
         <v>150</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>76</v>
@@ -2192,13 +2190,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="B22" s="4">
         <v>150</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>76</v>
@@ -2207,13 +2205,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="B23" s="4">
         <v>150</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>76</v>
@@ -2222,13 +2220,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B24" s="4">
         <v>150</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>76</v>
@@ -2237,228 +2235,18 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="B25" s="4">
         <v>150</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>76</v>
       </c>
       <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="4">
-        <v>150</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B27" s="4">
-        <v>150</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="4">
-        <v>150</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="4">
-        <v>150</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="4">
-        <v>150</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E30" s="4"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="4">
-        <v>150</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E31" s="4"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B32" s="4">
-        <v>150</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B33" s="4">
-        <v>150</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E33" s="4"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B34" s="4">
-        <v>150</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" s="4">
-        <v>150</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="4">
-        <v>150</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" s="4">
-        <v>150</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E37" s="4"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" s="4">
-        <v>150</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B39" s="4">
-        <v>150</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E39" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2470,7 +2258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18853A0E-12C4-4CB3-A3B5-4468DED6D8CC}">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" zoomScale="129" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="129" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A64" activeCellId="24" sqref="A5:XFD5 A6:XFD6 A10:XFD10 A11:XFD11 A15:XFD15 A16:XFD16 A19:XFD19 A20:XFD20 A27:XFD27 A28:XFD28 A32:XFD32 A33:XFD33 A37:XFD37 A38:XFD38 A42:XFD42 A43:XFD43 A47:XFD47 A48:XFD48 A52:XFD52 A53:XFD53 A57:XFD57 A58:XFD58 A59:XFD59 A63:XFD63 A64:XFD64"/>
     </sheetView>
   </sheetViews>
@@ -3671,8 +3459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39814E6E-F23C-4A03-B08E-3AF6786DB611}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView zoomScale="129" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3888,7 +3676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F663681D-5D43-458B-B272-FD4D5F886455}">
   <dimension ref="A1:N314"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="106" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Spike sorting with wave_clus and other functions
</commit_message>
<xml_diff>
--- a/metadata/mecp2RecordingsListNew.xlsx
+++ b/metadata/mecp2RecordingsListNew.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATLAB\MEA-NAP\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0F7878-0B9E-4AE2-82E9-A665B075BC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE4C2FA-8385-4567-BDF5-A724428B0E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{CE5D0629-84EA-4DEB-B886-7B072FA3D434}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{CE5D0629-84EA-4DEB-B886-7B072FA3D434}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Post-stim" sheetId="6" r:id="rId5"/>
     <sheet name="Stim" sheetId="2" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="119">
   <si>
     <t>231101_Mutant_ALICO3_1_Baseline</t>
   </si>
@@ -359,6 +359,45 @@
   </si>
   <si>
     <t>Circular shift</t>
+  </si>
+  <si>
+    <t>240209_MOS_ALICO1_9_patternstim</t>
+  </si>
+  <si>
+    <t>240209_MT_ALICO7_6_patternstim</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>240209_WT_ALICO3_2_patternstim</t>
+  </si>
+  <si>
+    <t>WT</t>
+  </si>
+  <si>
+    <t>240209_WT_ALICO3_3_patternstim_2</t>
+  </si>
+  <si>
+    <t>15, 51, 83</t>
+  </si>
+  <si>
+    <t>15, 51, 65, 78</t>
+  </si>
+  <si>
+    <t>15, 51</t>
+  </si>
+  <si>
+    <t>Stim did not run to end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pattern A stim did not run to end, </t>
+  </si>
+  <si>
+    <t>21, 32, 41, 52, 61, 72</t>
+  </si>
+  <si>
+    <t>22, 31, 42, 62, 71, 82</t>
   </si>
 </sst>
 </file>
@@ -466,9 +505,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -506,7 +545,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -612,7 +651,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -754,7 +793,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1861,8 +1900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF1FF9A-91A7-4CC9-B549-87D7B9661614}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="129" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A16" zoomScale="129" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3676,8 +3715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F663681D-5D43-458B-B272-FD4D5F886455}">
   <dimension ref="A1:N314"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4189,78 +4228,184 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
+      <c r="A14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14">
+        <v>250</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>117</v>
+      </c>
+      <c r="E14" t="s">
+        <v>118</v>
+      </c>
+      <c r="F14" t="s">
+        <v>114</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>200</v>
+      </c>
+      <c r="K14">
+        <v>200</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
+      <c r="A15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15">
+        <v>250</v>
+      </c>
+      <c r="C15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F15" t="s">
+        <v>113</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>200</v>
+      </c>
+      <c r="K15">
+        <v>200</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="2">
+        <v>250</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2">
+        <v>175</v>
+      </c>
+      <c r="K16" s="2">
+        <v>175</v>
+      </c>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="2">
+        <v>250</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2">
+        <v>175</v>
+      </c>
+      <c r="K17" s="2">
+        <v>175</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D32" s="6"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">

</xml_diff>